<commit_message>
Change final demand model aggregation
</commit_message>
<xml_diff>
--- a/project_exiobase/data/Eldata.xlsx
+++ b/project_exiobase/data/Eldata.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="79">
   <si>
     <t>i001</t>
   </si>
@@ -228,12 +228,6 @@
     <t>p058</t>
   </si>
   <si>
-    <t>FC</t>
-  </si>
-  <si>
-    <t>GCF</t>
-  </si>
-  <si>
     <t>elasIMP</t>
   </si>
   <si>
@@ -247,6 +241,18 @@
   </si>
   <si>
     <t>elasTOT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FCH  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">FCG  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">GFCF </t>
+  </si>
+  <si>
+    <t>INVCH</t>
   </si>
 </sst>
 </file>
@@ -586,10 +592,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -597,12 +603,12 @@
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -610,10 +616,26 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>71</v>
+        <v>76</v>
       </c>
       <c r="B3">
         <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>77</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>78</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -633,13 +655,13 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D1" t="s">
         <v>72</v>
-      </c>
-      <c r="C1" t="s">
-        <v>73</v>
-      </c>
-      <c r="D1" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -1150,7 +1172,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Add TFP parameter in production function
</commit_message>
<xml_diff>
--- a/project_exiobase/data/Eldata.xlsx
+++ b/project_exiobase/data/Eldata.xlsx
@@ -4,19 +4,20 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="90" windowWidth="20115" windowHeight="9780"/>
+    <workbookView xWindow="120" yWindow="90" windowWidth="20115" windowHeight="9780" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="elasFU" sheetId="5" r:id="rId1"/>
     <sheet name="elasTRADE" sheetId="8" r:id="rId2"/>
     <sheet name="elasPROD" sheetId="9" r:id="rId3"/>
+    <sheet name="TFP" sheetId="10" r:id="rId4"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="80">
   <si>
     <t>i001</t>
   </si>
@@ -253,6 +254,9 @@
   </si>
   <si>
     <t>INVCH</t>
+  </si>
+  <si>
+    <t>TFP</t>
   </si>
 </sst>
 </file>
@@ -594,7 +598,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
@@ -1458,4 +1462,302 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B36"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B36">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Change modeling of rest of the world
- there can only be one rest of the world region in the model
aggregation
- trade with rest of the world is shifted into the overall trade block.
now there is a distinction between total import (including from rest of
the world) and import from modeled regions
</commit_message>
<xml_diff>
--- a/project_exiobase/data/Eldata.xlsx
+++ b/project_exiobase/data/Eldata.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="90" windowWidth="20115" windowHeight="9780" activeTab="3"/>
+    <workbookView xWindow="120" yWindow="90" windowWidth="20115" windowHeight="9780" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="elasFU" sheetId="5" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="81">
   <si>
     <t>i001</t>
   </si>
@@ -229,9 +229,6 @@
     <t>p058</t>
   </si>
   <si>
-    <t>elasIMP</t>
-  </si>
-  <si>
     <t>elasIU_DM</t>
   </si>
   <si>
@@ -257,6 +254,12 @@
   </si>
   <si>
     <t>TFP</t>
+  </si>
+  <si>
+    <t>elasTRD</t>
+  </si>
+  <si>
+    <t>elasIMP_ROW</t>
   </si>
 </sst>
 </file>
@@ -607,12 +610,12 @@
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -620,7 +623,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -628,7 +631,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -636,7 +639,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B5">
         <v>0</v>
@@ -649,15 +652,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D36"/>
+  <dimension ref="A1:E36"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>70</v>
       </c>
@@ -665,10 +668,13 @@
         <v>71</v>
       </c>
       <c r="D1" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+        <v>80</v>
+      </c>
+      <c r="E1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>35</v>
       </c>
@@ -681,8 +687,11 @@
       <c r="D2">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>36</v>
       </c>
@@ -695,8 +704,11 @@
       <c r="D3">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>37</v>
       </c>
@@ -709,8 +721,11 @@
       <c r="D4">
         <v>5</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>38</v>
       </c>
@@ -723,8 +738,11 @@
       <c r="D5">
         <v>5</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>39</v>
       </c>
@@ -737,8 +755,11 @@
       <c r="D6">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>40</v>
       </c>
@@ -751,8 +772,11 @@
       <c r="D7">
         <v>5</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>41</v>
       </c>
@@ -765,8 +789,11 @@
       <c r="D8">
         <v>5</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>42</v>
       </c>
@@ -779,8 +806,11 @@
       <c r="D9">
         <v>5</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E9">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>43</v>
       </c>
@@ -793,8 +823,11 @@
       <c r="D10">
         <v>5</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E10">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>44</v>
       </c>
@@ -807,8 +840,11 @@
       <c r="D11">
         <v>5</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>45</v>
       </c>
@@ -821,8 +857,11 @@
       <c r="D12">
         <v>5</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E12">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>46</v>
       </c>
@@ -835,8 +874,11 @@
       <c r="D13">
         <v>5</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E13">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>47</v>
       </c>
@@ -849,8 +891,11 @@
       <c r="D14">
         <v>5</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E14">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>48</v>
       </c>
@@ -863,8 +908,11 @@
       <c r="D15">
         <v>5</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E15">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>49</v>
       </c>
@@ -877,8 +925,11 @@
       <c r="D16">
         <v>5</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E16">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>50</v>
       </c>
@@ -891,8 +942,11 @@
       <c r="D17">
         <v>5</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E17">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>51</v>
       </c>
@@ -905,8 +959,11 @@
       <c r="D18">
         <v>5</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E18">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>52</v>
       </c>
@@ -919,8 +976,11 @@
       <c r="D19">
         <v>5</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E19">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>53</v>
       </c>
@@ -933,8 +993,11 @@
       <c r="D20">
         <v>5</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E20">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>54</v>
       </c>
@@ -947,8 +1010,11 @@
       <c r="D21">
         <v>5</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E21">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>55</v>
       </c>
@@ -961,8 +1027,11 @@
       <c r="D22">
         <v>5</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E22">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>56</v>
       </c>
@@ -975,8 +1044,11 @@
       <c r="D23">
         <v>5</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E23">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>57</v>
       </c>
@@ -989,8 +1061,11 @@
       <c r="D24">
         <v>5</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E24">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>58</v>
       </c>
@@ -1003,8 +1078,11 @@
       <c r="D25">
         <v>5</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>59</v>
       </c>
@@ -1017,8 +1095,11 @@
       <c r="D26">
         <v>5</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E26">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>60</v>
       </c>
@@ -1031,8 +1112,11 @@
       <c r="D27">
         <v>5</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E27">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>61</v>
       </c>
@@ -1045,8 +1129,11 @@
       <c r="D28">
         <v>5</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E28">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>62</v>
       </c>
@@ -1059,8 +1146,11 @@
       <c r="D29">
         <v>5</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E29">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>63</v>
       </c>
@@ -1073,8 +1163,11 @@
       <c r="D30">
         <v>5</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E30">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>64</v>
       </c>
@@ -1087,8 +1180,11 @@
       <c r="D31">
         <v>5</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E31">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>65</v>
       </c>
@@ -1101,8 +1197,11 @@
       <c r="D32">
         <v>5</v>
       </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E32">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>66</v>
       </c>
@@ -1115,8 +1214,11 @@
       <c r="D33">
         <v>5</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E33">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>67</v>
       </c>
@@ -1129,8 +1231,11 @@
       <c r="D34">
         <v>5</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E34">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>68</v>
       </c>
@@ -1143,8 +1248,11 @@
       <c r="D35">
         <v>5</v>
       </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E35">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>69</v>
       </c>
@@ -1155,6 +1263,9 @@
         <v>5</v>
       </c>
       <c r="D36">
+        <v>5</v>
+      </c>
+      <c r="E36">
         <v>5</v>
       </c>
     </row>
@@ -1176,7 +1287,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -1468,13 +1579,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Introduce factor specific productivity parameter in the value added nest
</commit_message>
<xml_diff>
--- a/project_exiobase/data/Eldata.xlsx
+++ b/project_exiobase/data/Eldata.xlsx
@@ -4,20 +4,20 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="90" windowWidth="20115" windowHeight="9780" activeTab="1"/>
+    <workbookView xWindow="120" yWindow="90" windowWidth="20115" windowHeight="9780" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="elasFU" sheetId="5" r:id="rId1"/>
     <sheet name="elasTRADE" sheetId="8" r:id="rId2"/>
     <sheet name="elasPROD" sheetId="9" r:id="rId3"/>
-    <sheet name="TFP" sheetId="10" r:id="rId4"/>
+    <sheet name="FPROD" sheetId="10" r:id="rId4"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="82">
   <si>
     <t>i001</t>
   </si>
@@ -253,13 +253,16 @@
     <t>INVCH</t>
   </si>
   <si>
-    <t>TFP</t>
-  </si>
-  <si>
     <t>elasTRD</t>
   </si>
   <si>
     <t>elasIMP_ROW</t>
+  </si>
+  <si>
+    <t>COE</t>
+  </si>
+  <si>
+    <t>GOS</t>
   </si>
 </sst>
 </file>
@@ -654,8 +657,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -668,10 +671,10 @@
         <v>71</v>
       </c>
       <c r="D1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -1577,294 +1580,404 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B36"/>
+  <dimension ref="A1:C36"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+        <v>80</v>
+      </c>
+      <c r="C1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B3">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B4">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B5">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B6">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B7">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B8">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B9">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B10">
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B11">
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B12">
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B13">
         <v>1</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B14">
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B15">
         <v>1</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B16">
         <v>1</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B17">
         <v>1</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B18">
         <v>1</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>17</v>
       </c>
       <c r="B19">
         <v>1</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>18</v>
       </c>
       <c r="B20">
         <v>1</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>19</v>
       </c>
       <c r="B21">
         <v>1</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>20</v>
       </c>
       <c r="B22">
         <v>1</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>21</v>
       </c>
       <c r="B23">
         <v>1</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>22</v>
       </c>
       <c r="B24">
         <v>1</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>23</v>
       </c>
       <c r="B25">
         <v>1</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>24</v>
       </c>
       <c r="B26">
         <v>1</v>
       </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>25</v>
       </c>
       <c r="B27">
         <v>1</v>
       </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>26</v>
       </c>
       <c r="B28">
         <v>1</v>
       </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>27</v>
       </c>
       <c r="B29">
         <v>1</v>
       </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>28</v>
       </c>
       <c r="B30">
         <v>1</v>
       </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>29</v>
       </c>
       <c r="B31">
         <v>1</v>
       </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>30</v>
       </c>
       <c r="B32">
         <v>1</v>
       </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>31</v>
       </c>
       <c r="B33">
         <v>1</v>
       </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>32</v>
       </c>
       <c r="B34">
         <v>1</v>
       </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>33</v>
       </c>
       <c r="B35">
         <v>1</v>
       </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>34</v>
       </c>
       <c r="B36">
+        <v>1</v>
+      </c>
+      <c r="C36">
         <v>1</v>
       </c>
     </row>

</xml_diff>